<commit_message>
change_local and parse_pgn added
</commit_message>
<xml_diff>
--- a/data/otchet.xlsx
+++ b/data/otchet.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -567,12 +567,12 @@
     <row r="8">
       <c r="A8" s="9" t="inlineStr">
         <is>
-          <t>Играна во "2" туре 01.01.2000</t>
+          <t>Играна во "1" туре 01.01.2000</t>
         </is>
       </c>
       <c r="G8" s="9" t="inlineStr">
         <is>
-          <t>Играна во "2" туре 01.01.2000</t>
+          <t>Играна во "1" туре 01.01.2000</t>
         </is>
       </c>
     </row>
@@ -666,12 +666,12 @@
       </c>
       <c r="B13" s="10" t="inlineStr">
         <is>
-          <t>Bc4</t>
+          <t>Кf3</t>
         </is>
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>Bc5</t>
+          <t>Кc6</t>
         </is>
       </c>
       <c r="G13" s="8" t="n">
@@ -679,12 +679,12 @@
       </c>
       <c r="H13" s="10" t="inlineStr">
         <is>
-          <t>Bc4</t>
+          <t>Кf3</t>
         </is>
       </c>
       <c r="I13" s="10" t="inlineStr">
         <is>
-          <t>Bc5</t>
+          <t>Кc6</t>
         </is>
       </c>
     </row>
@@ -694,12 +694,12 @@
       </c>
       <c r="B14" s="10" t="inlineStr">
         <is>
-          <t>Nf3</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="C14" s="10" t="inlineStr">
         <is>
-          <t>Nc6</t>
+          <t>f6</t>
         </is>
       </c>
       <c r="G14" s="8" t="n">
@@ -707,12 +707,12 @@
       </c>
       <c r="H14" s="10" t="inlineStr">
         <is>
-          <t>Nf3</t>
+          <t>c3</t>
         </is>
       </c>
       <c r="I14" s="10" t="inlineStr">
         <is>
-          <t>Nc6</t>
+          <t>d6</t>
         </is>
       </c>
     </row>
@@ -722,12 +722,12 @@
       </c>
       <c r="B15" s="10" t="inlineStr">
         <is>
-          <t>Ng5</t>
+          <t>d5</t>
         </is>
       </c>
       <c r="C15" s="10" t="inlineStr">
         <is>
-          <t>Qxg5</t>
+          <t>Кd4</t>
         </is>
       </c>
       <c r="G15" s="8" t="n">
@@ -735,12 +735,12 @@
       </c>
       <c r="H15" s="10" t="inlineStr">
         <is>
-          <t>Ng5</t>
+          <t>d4</t>
         </is>
       </c>
       <c r="I15" s="10" t="inlineStr">
         <is>
-          <t>Qxg5</t>
+          <t>Cg4</t>
         </is>
       </c>
     </row>
@@ -750,12 +750,12 @@
       </c>
       <c r="B16" s="10" t="inlineStr">
         <is>
-          <t>d3</t>
+          <t>Кxd4</t>
         </is>
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>Qxg2</t>
+          <t>exd4</t>
         </is>
       </c>
       <c r="G16" s="8" t="n">
@@ -763,12 +763,12 @@
       </c>
       <c r="H16" s="10" t="inlineStr">
         <is>
-          <t>d3</t>
+          <t>Cg5</t>
         </is>
       </c>
       <c r="I16" s="10" t="inlineStr">
         <is>
-          <t>Qxg2</t>
+          <t>f6</t>
         </is>
       </c>
     </row>
@@ -778,12 +778,12 @@
       </c>
       <c r="B17" s="10" t="inlineStr">
         <is>
-          <t>Qe2</t>
+          <t>Фxd4</t>
         </is>
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>Qxh1+</t>
+          <t>d6</t>
         </is>
       </c>
       <c r="G17" s="8" t="n">
@@ -791,12 +791,12 @@
       </c>
       <c r="H17" s="10" t="inlineStr">
         <is>
-          <t>Qe2</t>
+          <t>Ce3</t>
         </is>
       </c>
       <c r="I17" s="10" t="inlineStr">
         <is>
-          <t>Qxh1+</t>
+          <t>Фd7</t>
         </is>
       </c>
     </row>
@@ -806,12 +806,12 @@
       </c>
       <c r="B18" s="10" t="inlineStr">
         <is>
-          <t>Qf1</t>
+          <t>Кc3</t>
         </is>
       </c>
       <c r="C18" s="10" t="inlineStr">
         <is>
-          <t>Qf3</t>
+          <t>f5</t>
         </is>
       </c>
       <c r="G18" s="8" t="n">
@@ -819,12 +819,12 @@
       </c>
       <c r="H18" s="10" t="inlineStr">
         <is>
-          <t>Qf1</t>
+          <t>Кbd2</t>
         </is>
       </c>
       <c r="I18" s="10" t="inlineStr">
         <is>
-          <t>Qf3</t>
+          <t>O-O-O</t>
         </is>
       </c>
     </row>
@@ -834,12 +834,12 @@
       </c>
       <c r="B19" s="10" t="inlineStr">
         <is>
-          <t>Nd2</t>
+          <t>e5</t>
         </is>
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>Qg4</t>
+          <t>dxe5</t>
         </is>
       </c>
       <c r="G19" s="8" t="n">
@@ -847,12 +847,12 @@
       </c>
       <c r="H19" s="10" t="inlineStr">
         <is>
-          <t>Nd2</t>
+          <t>h3</t>
         </is>
       </c>
       <c r="I19" s="10" t="inlineStr">
         <is>
-          <t>Qg4</t>
+          <t>Cxf3</t>
         </is>
       </c>
     </row>
@@ -862,12 +862,12 @@
       </c>
       <c r="B20" s="10" t="inlineStr">
         <is>
-          <t>a3</t>
+          <t>Фxe5+</t>
         </is>
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>Nd4</t>
+          <t>Фe7</t>
         </is>
       </c>
       <c r="G20" s="8" t="n">
@@ -875,12 +875,12 @@
       </c>
       <c r="H20" s="10" t="inlineStr">
         <is>
-          <t>a3</t>
+          <t>Фxf3</t>
         </is>
       </c>
       <c r="I20" s="10" t="inlineStr">
         <is>
-          <t>Nd4</t>
+          <t>Кge7</t>
         </is>
       </c>
     </row>
@@ -890,12 +890,12 @@
       </c>
       <c r="B21" s="10" t="inlineStr">
         <is>
-          <t>b4</t>
+          <t>Фxe7+</t>
         </is>
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>Nxc2#</t>
+          <t>Кxe7</t>
         </is>
       </c>
       <c r="G21" s="8" t="n">
@@ -903,12 +903,12 @@
       </c>
       <c r="H21" s="10" t="inlineStr">
         <is>
-          <t>b4</t>
+          <t>d5</t>
         </is>
       </c>
       <c r="I21" s="10" t="inlineStr">
         <is>
-          <t>Nxc2#</t>
+          <t>Фf7</t>
         </is>
       </c>
     </row>
@@ -916,182 +916,632 @@
       <c r="A22" s="8" t="n">
         <v>11</v>
       </c>
+      <c r="B22" s="10" t="inlineStr">
+        <is>
+          <t>Cd3</t>
+        </is>
+      </c>
+      <c r="C22" s="10" t="inlineStr">
+        <is>
+          <t>c6</t>
+        </is>
+      </c>
       <c r="G22" s="8" t="n">
         <v>11</v>
+      </c>
+      <c r="H22" s="10" t="inlineStr">
+        <is>
+          <t>dxc6</t>
+        </is>
+      </c>
+      <c r="I22" s="10" t="inlineStr">
+        <is>
+          <t>Кxc6</t>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="8" t="n">
         <v>12</v>
       </c>
+      <c r="B23" s="10" t="inlineStr">
+        <is>
+          <t>O-O</t>
+        </is>
+      </c>
+      <c r="C23" s="10" t="inlineStr">
+        <is>
+          <t>Кxd5</t>
+        </is>
+      </c>
       <c r="G23" s="8" t="n">
         <v>12</v>
+      </c>
+      <c r="H23" s="10" t="inlineStr">
+        <is>
+          <t>Cxa7</t>
+        </is>
+      </c>
+      <c r="I23" s="10" t="inlineStr">
+        <is>
+          <t>Кxa7</t>
+        </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="8" t="n">
         <v>13</v>
       </c>
+      <c r="B24" s="10" t="inlineStr">
+        <is>
+          <t>Лe1+</t>
+        </is>
+      </c>
+      <c r="C24" s="10" t="inlineStr">
+        <is>
+          <t>Ce7</t>
+        </is>
+      </c>
       <c r="G24" s="8" t="n">
         <v>13</v>
+      </c>
+      <c r="H24" s="10" t="inlineStr">
+        <is>
+          <t>g4</t>
+        </is>
+      </c>
+      <c r="I24" s="10" t="inlineStr">
+        <is>
+          <t>d5</t>
+        </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="8" t="n">
         <v>14</v>
       </c>
+      <c r="B25" s="10" t="inlineStr">
+        <is>
+          <t>Кxd5</t>
+        </is>
+      </c>
+      <c r="C25" s="10" t="inlineStr">
+        <is>
+          <t>cxd5</t>
+        </is>
+      </c>
       <c r="G25" s="8" t="n">
         <v>14</v>
+      </c>
+      <c r="H25" s="10" t="inlineStr">
+        <is>
+          <t>exd5</t>
+        </is>
+      </c>
+      <c r="I25" s="10" t="inlineStr">
+        <is>
+          <t>Лxd5</t>
+        </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="8" t="n">
         <v>15</v>
       </c>
+      <c r="B26" s="10" t="inlineStr">
+        <is>
+          <t>h3</t>
+        </is>
+      </c>
+      <c r="C26" s="10" t="inlineStr">
+        <is>
+          <t>Ce6</t>
+        </is>
+      </c>
       <c r="G26" s="8" t="n">
         <v>15</v>
+      </c>
+      <c r="H26" s="10" t="inlineStr">
+        <is>
+          <t>Лd1</t>
+        </is>
+      </c>
+      <c r="I26" s="10" t="inlineStr">
+        <is>
+          <t>Лc5</t>
+        </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="8" t="n">
         <v>16</v>
       </c>
+      <c r="B27" s="10" t="inlineStr">
+        <is>
+          <t>Лxe6</t>
+        </is>
+      </c>
+      <c r="C27" s="10" t="inlineStr">
+        <is>
+          <t>O-O-O</t>
+        </is>
+      </c>
       <c r="G27" s="8" t="n">
         <v>16</v>
+      </c>
+      <c r="H27" s="10" t="inlineStr">
+        <is>
+          <t>Фd3</t>
+        </is>
+      </c>
+      <c r="I27" s="10" t="inlineStr">
+        <is>
+          <t>Cd6</t>
+        </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="8" t="n">
         <v>17</v>
       </c>
+      <c r="B28" s="10" t="inlineStr">
+        <is>
+          <t>Лxe7</t>
+        </is>
+      </c>
+      <c r="C28" s="10" t="inlineStr">
+        <is>
+          <t>Лhe8</t>
+        </is>
+      </c>
       <c r="G28" s="8" t="n">
         <v>17</v>
+      </c>
+      <c r="H28" s="10" t="inlineStr">
+        <is>
+          <t>Фf5+</t>
+        </is>
+      </c>
+      <c r="I28" s="10" t="inlineStr">
+        <is>
+          <t>Крb8</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="8" t="n">
         <v>18</v>
       </c>
+      <c r="B29" s="10" t="inlineStr">
+        <is>
+          <t>Лxg7</t>
+        </is>
+      </c>
+      <c r="C29" s="10" t="inlineStr">
+        <is>
+          <t>Лe1+</t>
+        </is>
+      </c>
       <c r="G29" s="8" t="n">
         <v>18</v>
+      </c>
+      <c r="H29" s="10" t="inlineStr">
+        <is>
+          <t>b4</t>
+        </is>
+      </c>
+      <c r="I29" s="10" t="inlineStr">
+        <is>
+          <t>Лxc4</t>
+        </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="8" t="n">
         <v>19</v>
       </c>
+      <c r="B30" s="10" t="inlineStr">
+        <is>
+          <t>Крh2</t>
+        </is>
+      </c>
+      <c r="C30" s="10" t="inlineStr">
+        <is>
+          <t>h5</t>
+        </is>
+      </c>
       <c r="G30" s="8" t="n">
         <v>19</v>
+      </c>
+      <c r="H30" s="10" t="inlineStr">
+        <is>
+          <t>Cxc4</t>
+        </is>
+      </c>
+      <c r="I30" s="10" t="inlineStr">
+        <is>
+          <t>Фxc4</t>
+        </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="8" t="n">
         <v>20</v>
       </c>
+      <c r="B31" s="10" t="inlineStr">
+        <is>
+          <t>Cxf5+</t>
+        </is>
+      </c>
+      <c r="C31" s="10" t="inlineStr">
+        <is>
+          <t>Крb8</t>
+        </is>
+      </c>
       <c r="G31" s="8" t="n">
         <v>20</v>
+      </c>
+      <c r="H31" s="10" t="inlineStr">
+        <is>
+          <t>Крe2</t>
+        </is>
+      </c>
+      <c r="I31" s="10" t="inlineStr">
+        <is>
+          <t>Фxa3</t>
+        </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="8" t="n">
         <v>21</v>
       </c>
+      <c r="B32" s="10" t="inlineStr">
+        <is>
+          <t>Лg5</t>
+        </is>
+      </c>
+      <c r="C32" s="10" t="inlineStr">
+        <is>
+          <t>Лh8</t>
+        </is>
+      </c>
       <c r="G32" s="8" t="n">
         <v>21</v>
+      </c>
+      <c r="H32" s="10" t="inlineStr">
+        <is>
+          <t>Фe4</t>
+        </is>
+      </c>
+      <c r="I32" s="10" t="inlineStr">
+        <is>
+          <t>Фxb4</t>
+        </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="8" t="n">
         <v>22</v>
       </c>
+      <c r="B33" s="10" t="inlineStr">
+        <is>
+          <t>b3</t>
+        </is>
+      </c>
+      <c r="C33" s="10" t="inlineStr">
+        <is>
+          <t>d4</t>
+        </is>
+      </c>
       <c r="G33" s="8" t="n">
         <v>22</v>
+      </c>
+      <c r="H33" s="10" t="inlineStr">
+        <is>
+          <t>Фe3</t>
+        </is>
+      </c>
+      <c r="I33" s="10" t="inlineStr">
+        <is>
+          <t>Фb5+</t>
+        </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="8" t="n">
         <v>23</v>
       </c>
+      <c r="B34" s="10" t="inlineStr">
+        <is>
+          <t>Cb2</t>
+        </is>
+      </c>
+      <c r="C34" s="10" t="inlineStr">
+        <is>
+          <t>Лxa1</t>
+        </is>
+      </c>
       <c r="G34" s="8" t="n">
         <v>23</v>
+      </c>
+      <c r="H34" s="10" t="inlineStr">
+        <is>
+          <t>Крf3</t>
+        </is>
+      </c>
+      <c r="I34" s="10" t="inlineStr">
+        <is>
+          <t>Cc5</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="8" t="n">
         <v>24</v>
       </c>
+      <c r="B35" s="10" t="inlineStr">
+        <is>
+          <t>Cxa1</t>
+        </is>
+      </c>
+      <c r="C35" s="10" t="inlineStr">
+        <is>
+          <t>d3</t>
+        </is>
+      </c>
       <c r="G35" s="8" t="n">
         <v>24</v>
+      </c>
+      <c r="H35" s="10" t="inlineStr">
+        <is>
+          <t>Фa3</t>
+        </is>
+      </c>
+      <c r="I35" s="10" t="inlineStr">
+        <is>
+          <t>Cxa3</t>
+        </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="8" t="n">
         <v>25</v>
       </c>
+      <c r="B36" s="10" t="inlineStr">
+        <is>
+          <t>cxd3</t>
+        </is>
+      </c>
+      <c r="C36" s="10" t="inlineStr">
+        <is>
+          <t>h4</t>
+        </is>
+      </c>
       <c r="G36" s="8" t="n">
         <v>25</v>
+      </c>
+      <c r="H36" s="10" t="inlineStr">
+        <is>
+          <t>Крg3</t>
+        </is>
+      </c>
+      <c r="I36" s="10" t="inlineStr">
+        <is>
+          <t>Фc3+</t>
+        </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="8" t="n">
         <v>26</v>
       </c>
+      <c r="B37" s="10" t="inlineStr">
+        <is>
+          <t>d4</t>
+        </is>
+      </c>
+      <c r="C37" s="10" t="inlineStr">
+        <is>
+          <t>Лf8</t>
+        </is>
+      </c>
       <c r="G37" s="8" t="n">
         <v>26</v>
+      </c>
+      <c r="H37" s="10" t="inlineStr">
+        <is>
+          <t>f3</t>
+        </is>
+      </c>
+      <c r="I37" s="10" t="inlineStr">
+        <is>
+          <t>Фxd2</t>
+        </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="8" t="n">
         <v>27</v>
       </c>
+      <c r="B38" s="10" t="inlineStr">
+        <is>
+          <t>d5</t>
+        </is>
+      </c>
+      <c r="C38" s="10" t="inlineStr">
+        <is>
+          <t>Крc7</t>
+        </is>
+      </c>
       <c r="G38" s="8" t="n">
         <v>27</v>
+      </c>
+      <c r="H38" s="10" t="inlineStr">
+        <is>
+          <t>f4</t>
+        </is>
+      </c>
+      <c r="I38" s="10" t="inlineStr">
+        <is>
+          <t>Фe3+</t>
+        </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="8" t="n">
         <v>28</v>
       </c>
+      <c r="B39" s="10" t="inlineStr">
+        <is>
+          <t>Ce5+</t>
+        </is>
+      </c>
+      <c r="C39" s="10" t="inlineStr">
+        <is>
+          <t>Крb6</t>
+        </is>
+      </c>
       <c r="G39" s="8" t="n">
         <v>28</v>
+      </c>
+      <c r="H39" s="10" t="inlineStr">
+        <is>
+          <t>Крh4</t>
+        </is>
+      </c>
+      <c r="I39" s="10" t="inlineStr">
+        <is>
+          <t>Фxf4</t>
+        </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="8" t="n">
         <v>29</v>
       </c>
+      <c r="B40" s="10" t="inlineStr">
+        <is>
+          <t>Cd4+</t>
+        </is>
+      </c>
+      <c r="C40" s="10" t="inlineStr">
+        <is>
+          <t>Крc7</t>
+        </is>
+      </c>
       <c r="G40" s="8" t="n">
         <v>29</v>
+      </c>
+      <c r="H40" s="10" t="inlineStr">
+        <is>
+          <t>Крh5</t>
+        </is>
+      </c>
+      <c r="I40" s="10" t="inlineStr">
+        <is>
+          <t>g6+</t>
+        </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="8" t="n">
         <v>30</v>
       </c>
+      <c r="B41" s="10" t="inlineStr">
+        <is>
+          <t>Cg7</t>
+        </is>
+      </c>
+      <c r="C41" s="10" t="inlineStr">
+        <is>
+          <t>Лf7</t>
+        </is>
+      </c>
       <c r="G41" s="8" t="n">
         <v>30</v>
+      </c>
+      <c r="H41" s="10" t="inlineStr">
+        <is>
+          <t>Крh4</t>
+        </is>
+      </c>
+      <c r="I41" s="10" t="inlineStr">
+        <is>
+          <t>g5+</t>
+        </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="8" t="n">
         <v>31</v>
       </c>
+      <c r="B42" s="10" t="inlineStr">
+        <is>
+          <t>g4</t>
+        </is>
+      </c>
+      <c r="C42" s="10" t="inlineStr">
+        <is>
+          <t>Крd6</t>
+        </is>
+      </c>
       <c r="G42" s="8" t="n">
         <v>31</v>
+      </c>
+      <c r="H42" s="10" t="inlineStr">
+        <is>
+          <t>Крh5</t>
+        </is>
+      </c>
+      <c r="I42" s="10" t="inlineStr">
+        <is>
+          <t>Фg3</t>
+        </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="8" t="n">
         <v>32</v>
       </c>
+      <c r="B43" s="10" t="inlineStr">
+        <is>
+          <t>Ca1</t>
+        </is>
+      </c>
+      <c r="C43" s="10" t="inlineStr">
+        <is>
+          <t>Крxd5</t>
+        </is>
+      </c>
       <c r="G43" s="8" t="n">
         <v>32</v>
+      </c>
+      <c r="H43" s="10" t="inlineStr">
+        <is>
+          <t>Лd1</t>
+        </is>
+      </c>
+      <c r="I43" s="10" t="inlineStr">
+        <is>
+          <t>Фxh3#</t>
+        </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="8" t="n">
         <v>33</v>
       </c>
+      <c r="B44" s="10" t="inlineStr">
+        <is>
+          <t>Лh5</t>
+        </is>
+      </c>
+      <c r="C44" s="10" t="inlineStr">
+        <is>
+          <t>Лe7</t>
+        </is>
+      </c>
       <c r="G44" s="8" t="n">
         <v>33</v>
       </c>
@@ -1100,6 +1550,16 @@
       <c r="A45" s="8" t="n">
         <v>34</v>
       </c>
+      <c r="B45" s="10" t="inlineStr">
+        <is>
+          <t>Лxh4</t>
+        </is>
+      </c>
+      <c r="C45" s="10" t="inlineStr">
+        <is>
+          <t>Лe2</t>
+        </is>
+      </c>
       <c r="G45" s="8" t="n">
         <v>34</v>
       </c>
@@ -1108,6 +1568,16 @@
       <c r="A46" s="8" t="n">
         <v>35</v>
       </c>
+      <c r="B46" s="10" t="inlineStr">
+        <is>
+          <t>Крg3</t>
+        </is>
+      </c>
+      <c r="C46" s="10" t="inlineStr">
+        <is>
+          <t>Лxa2</t>
+        </is>
+      </c>
       <c r="G46" s="8" t="n">
         <v>35</v>
       </c>
@@ -1115,6 +1585,16 @@
     <row r="47">
       <c r="A47" s="8" t="n">
         <v>36</v>
+      </c>
+      <c r="B47" s="10" t="inlineStr">
+        <is>
+          <t>Ch8</t>
+        </is>
+      </c>
+      <c r="C47" s="10" t="inlineStr">
+        <is>
+          <t>Лa3</t>
+        </is>
       </c>
       <c r="G47" s="8" t="n">
         <v>36</v>

</xml_diff>

<commit_message>
Added the ability to select localization. Added examples for the .txt format.
</commit_message>
<xml_diff>
--- a/data/otchet.xlsx
+++ b/data/otchet.xlsx
@@ -666,12 +666,12 @@
       </c>
       <c r="B13" s="10" t="inlineStr">
         <is>
-          <t>Кf3</t>
+          <t>Nf3</t>
         </is>
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>Кc6</t>
+          <t>Nc6</t>
         </is>
       </c>
       <c r="G13" s="8" t="n">
@@ -679,12 +679,12 @@
       </c>
       <c r="H13" s="10" t="inlineStr">
         <is>
-          <t>Кf3</t>
+          <t>Nf3</t>
         </is>
       </c>
       <c r="I13" s="10" t="inlineStr">
         <is>
-          <t>Кc6</t>
+          <t>Nc6</t>
         </is>
       </c>
     </row>
@@ -727,7 +727,7 @@
       </c>
       <c r="C15" s="10" t="inlineStr">
         <is>
-          <t>Кd4</t>
+          <t>Nd4</t>
         </is>
       </c>
       <c r="G15" s="8" t="n">
@@ -740,7 +740,7 @@
       </c>
       <c r="I15" s="10" t="inlineStr">
         <is>
-          <t>Cg4</t>
+          <t>Bg4</t>
         </is>
       </c>
     </row>
@@ -750,7 +750,7 @@
       </c>
       <c r="B16" s="10" t="inlineStr">
         <is>
-          <t>Кxd4</t>
+          <t>Nxd4</t>
         </is>
       </c>
       <c r="C16" s="10" t="inlineStr">
@@ -763,7 +763,7 @@
       </c>
       <c r="H16" s="10" t="inlineStr">
         <is>
-          <t>Cg5</t>
+          <t>Bg5</t>
         </is>
       </c>
       <c r="I16" s="10" t="inlineStr">
@@ -778,7 +778,7 @@
       </c>
       <c r="B17" s="10" t="inlineStr">
         <is>
-          <t>Фxd4</t>
+          <t>Qxd4</t>
         </is>
       </c>
       <c r="C17" s="10" t="inlineStr">
@@ -791,12 +791,12 @@
       </c>
       <c r="H17" s="10" t="inlineStr">
         <is>
-          <t>Ce3</t>
+          <t>Be3</t>
         </is>
       </c>
       <c r="I17" s="10" t="inlineStr">
         <is>
-          <t>Фd7</t>
+          <t>Qd7</t>
         </is>
       </c>
     </row>
@@ -806,7 +806,7 @@
       </c>
       <c r="B18" s="10" t="inlineStr">
         <is>
-          <t>Кc3</t>
+          <t>Nc3</t>
         </is>
       </c>
       <c r="C18" s="10" t="inlineStr">
@@ -819,7 +819,7 @@
       </c>
       <c r="H18" s="10" t="inlineStr">
         <is>
-          <t>Кbd2</t>
+          <t>Nbd2</t>
         </is>
       </c>
       <c r="I18" s="10" t="inlineStr">
@@ -852,7 +852,7 @@
       </c>
       <c r="I19" s="10" t="inlineStr">
         <is>
-          <t>Cxf3</t>
+          <t>Bxf3</t>
         </is>
       </c>
     </row>
@@ -862,12 +862,12 @@
       </c>
       <c r="B20" s="10" t="inlineStr">
         <is>
-          <t>Фxe5+</t>
+          <t>Qxe5+</t>
         </is>
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>Фe7</t>
+          <t>Qe7</t>
         </is>
       </c>
       <c r="G20" s="8" t="n">
@@ -875,12 +875,12 @@
       </c>
       <c r="H20" s="10" t="inlineStr">
         <is>
-          <t>Фxf3</t>
+          <t>Qxf3</t>
         </is>
       </c>
       <c r="I20" s="10" t="inlineStr">
         <is>
-          <t>Кge7</t>
+          <t>Nge7</t>
         </is>
       </c>
     </row>
@@ -890,12 +890,12 @@
       </c>
       <c r="B21" s="10" t="inlineStr">
         <is>
-          <t>Фxe7+</t>
+          <t>Qxe7+</t>
         </is>
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>Кxe7</t>
+          <t>Nxe7</t>
         </is>
       </c>
       <c r="G21" s="8" t="n">
@@ -908,7 +908,7 @@
       </c>
       <c r="I21" s="10" t="inlineStr">
         <is>
-          <t>Фf7</t>
+          <t>Qf7</t>
         </is>
       </c>
     </row>
@@ -918,7 +918,7 @@
       </c>
       <c r="B22" s="10" t="inlineStr">
         <is>
-          <t>Cd3</t>
+          <t>Bd3</t>
         </is>
       </c>
       <c r="C22" s="10" t="inlineStr">
@@ -936,7 +936,7 @@
       </c>
       <c r="I22" s="10" t="inlineStr">
         <is>
-          <t>Кxc6</t>
+          <t>Nxc6</t>
         </is>
       </c>
     </row>
@@ -951,7 +951,7 @@
       </c>
       <c r="C23" s="10" t="inlineStr">
         <is>
-          <t>Кxd5</t>
+          <t>Nxd5</t>
         </is>
       </c>
       <c r="G23" s="8" t="n">
@@ -959,12 +959,12 @@
       </c>
       <c r="H23" s="10" t="inlineStr">
         <is>
-          <t>Cxa7</t>
+          <t>Bxa7</t>
         </is>
       </c>
       <c r="I23" s="10" t="inlineStr">
         <is>
-          <t>Кxa7</t>
+          <t>Nxa7</t>
         </is>
       </c>
     </row>
@@ -974,12 +974,12 @@
       </c>
       <c r="B24" s="10" t="inlineStr">
         <is>
-          <t>Лe1+</t>
+          <t>Re1+</t>
         </is>
       </c>
       <c r="C24" s="10" t="inlineStr">
         <is>
-          <t>Ce7</t>
+          <t>Be7</t>
         </is>
       </c>
       <c r="G24" s="8" t="n">
@@ -1002,7 +1002,7 @@
       </c>
       <c r="B25" s="10" t="inlineStr">
         <is>
-          <t>Кxd5</t>
+          <t>Nxd5</t>
         </is>
       </c>
       <c r="C25" s="10" t="inlineStr">
@@ -1020,7 +1020,7 @@
       </c>
       <c r="I25" s="10" t="inlineStr">
         <is>
-          <t>Лxd5</t>
+          <t>Rxd5</t>
         </is>
       </c>
     </row>
@@ -1035,7 +1035,7 @@
       </c>
       <c r="C26" s="10" t="inlineStr">
         <is>
-          <t>Ce6</t>
+          <t>Be6</t>
         </is>
       </c>
       <c r="G26" s="8" t="n">
@@ -1043,12 +1043,12 @@
       </c>
       <c r="H26" s="10" t="inlineStr">
         <is>
-          <t>Лd1</t>
+          <t>Rd1</t>
         </is>
       </c>
       <c r="I26" s="10" t="inlineStr">
         <is>
-          <t>Лc5</t>
+          <t>Rc5</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="B27" s="10" t="inlineStr">
         <is>
-          <t>Лxe6</t>
+          <t>Rxe6</t>
         </is>
       </c>
       <c r="C27" s="10" t="inlineStr">
@@ -1071,12 +1071,12 @@
       </c>
       <c r="H27" s="10" t="inlineStr">
         <is>
-          <t>Фd3</t>
+          <t>Qd3</t>
         </is>
       </c>
       <c r="I27" s="10" t="inlineStr">
         <is>
-          <t>Cd6</t>
+          <t>Bd6</t>
         </is>
       </c>
     </row>
@@ -1086,12 +1086,12 @@
       </c>
       <c r="B28" s="10" t="inlineStr">
         <is>
-          <t>Лxe7</t>
+          <t>Rxe7</t>
         </is>
       </c>
       <c r="C28" s="10" t="inlineStr">
         <is>
-          <t>Лhe8</t>
+          <t>Rhe8</t>
         </is>
       </c>
       <c r="G28" s="8" t="n">
@@ -1099,12 +1099,12 @@
       </c>
       <c r="H28" s="10" t="inlineStr">
         <is>
-          <t>Фf5+</t>
+          <t>Qf5+</t>
         </is>
       </c>
       <c r="I28" s="10" t="inlineStr">
         <is>
-          <t>Крb8</t>
+          <t>Kb8</t>
         </is>
       </c>
     </row>
@@ -1114,12 +1114,12 @@
       </c>
       <c r="B29" s="10" t="inlineStr">
         <is>
-          <t>Лxg7</t>
+          <t>Rxg7</t>
         </is>
       </c>
       <c r="C29" s="10" t="inlineStr">
         <is>
-          <t>Лe1+</t>
+          <t>Re1+</t>
         </is>
       </c>
       <c r="G29" s="8" t="n">
@@ -1132,7 +1132,7 @@
       </c>
       <c r="I29" s="10" t="inlineStr">
         <is>
-          <t>Лxc4</t>
+          <t>Rxc4</t>
         </is>
       </c>
     </row>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="B30" s="10" t="inlineStr">
         <is>
-          <t>Крh2</t>
+          <t>Kh2</t>
         </is>
       </c>
       <c r="C30" s="10" t="inlineStr">
@@ -1155,12 +1155,12 @@
       </c>
       <c r="H30" s="10" t="inlineStr">
         <is>
-          <t>Cxc4</t>
+          <t>Bxc4</t>
         </is>
       </c>
       <c r="I30" s="10" t="inlineStr">
         <is>
-          <t>Фxc4</t>
+          <t>Qxc4</t>
         </is>
       </c>
     </row>
@@ -1170,12 +1170,12 @@
       </c>
       <c r="B31" s="10" t="inlineStr">
         <is>
-          <t>Cxf5+</t>
+          <t>Bxf5+</t>
         </is>
       </c>
       <c r="C31" s="10" t="inlineStr">
         <is>
-          <t>Крb8</t>
+          <t>Kb8</t>
         </is>
       </c>
       <c r="G31" s="8" t="n">
@@ -1183,12 +1183,12 @@
       </c>
       <c r="H31" s="10" t="inlineStr">
         <is>
-          <t>Крe2</t>
+          <t>Ke2</t>
         </is>
       </c>
       <c r="I31" s="10" t="inlineStr">
         <is>
-          <t>Фxa3</t>
+          <t>Qxa3</t>
         </is>
       </c>
     </row>
@@ -1198,12 +1198,12 @@
       </c>
       <c r="B32" s="10" t="inlineStr">
         <is>
-          <t>Лg5</t>
+          <t>Rg5</t>
         </is>
       </c>
       <c r="C32" s="10" t="inlineStr">
         <is>
-          <t>Лh8</t>
+          <t>Rh8</t>
         </is>
       </c>
       <c r="G32" s="8" t="n">
@@ -1211,12 +1211,12 @@
       </c>
       <c r="H32" s="10" t="inlineStr">
         <is>
-          <t>Фe4</t>
+          <t>Qe4</t>
         </is>
       </c>
       <c r="I32" s="10" t="inlineStr">
         <is>
-          <t>Фxb4</t>
+          <t>Qxb4</t>
         </is>
       </c>
     </row>
@@ -1239,12 +1239,12 @@
       </c>
       <c r="H33" s="10" t="inlineStr">
         <is>
-          <t>Фe3</t>
+          <t>Qe3</t>
         </is>
       </c>
       <c r="I33" s="10" t="inlineStr">
         <is>
-          <t>Фb5+</t>
+          <t>Qb5+</t>
         </is>
       </c>
     </row>
@@ -1254,12 +1254,12 @@
       </c>
       <c r="B34" s="10" t="inlineStr">
         <is>
-          <t>Cb2</t>
+          <t>Bb2</t>
         </is>
       </c>
       <c r="C34" s="10" t="inlineStr">
         <is>
-          <t>Лxa1</t>
+          <t>Rxa1</t>
         </is>
       </c>
       <c r="G34" s="8" t="n">
@@ -1267,12 +1267,12 @@
       </c>
       <c r="H34" s="10" t="inlineStr">
         <is>
-          <t>Крf3</t>
+          <t>Kf3</t>
         </is>
       </c>
       <c r="I34" s="10" t="inlineStr">
         <is>
-          <t>Cc5</t>
+          <t>Bc5</t>
         </is>
       </c>
     </row>
@@ -1282,7 +1282,7 @@
       </c>
       <c r="B35" s="10" t="inlineStr">
         <is>
-          <t>Cxa1</t>
+          <t>Bxa1</t>
         </is>
       </c>
       <c r="C35" s="10" t="inlineStr">
@@ -1295,12 +1295,12 @@
       </c>
       <c r="H35" s="10" t="inlineStr">
         <is>
-          <t>Фa3</t>
+          <t>Qa3</t>
         </is>
       </c>
       <c r="I35" s="10" t="inlineStr">
         <is>
-          <t>Cxa3</t>
+          <t>Bxa3</t>
         </is>
       </c>
     </row>
@@ -1323,12 +1323,12 @@
       </c>
       <c r="H36" s="10" t="inlineStr">
         <is>
-          <t>Крg3</t>
+          <t>Kg3</t>
         </is>
       </c>
       <c r="I36" s="10" t="inlineStr">
         <is>
-          <t>Фc3+</t>
+          <t>Qc3+</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="C37" s="10" t="inlineStr">
         <is>
-          <t>Лf8</t>
+          <t>Rf8</t>
         </is>
       </c>
       <c r="G37" s="8" t="n">
@@ -1356,7 +1356,7 @@
       </c>
       <c r="I37" s="10" t="inlineStr">
         <is>
-          <t>Фxd2</t>
+          <t>Qxd2</t>
         </is>
       </c>
     </row>
@@ -1371,7 +1371,7 @@
       </c>
       <c r="C38" s="10" t="inlineStr">
         <is>
-          <t>Крc7</t>
+          <t>Kc7</t>
         </is>
       </c>
       <c r="G38" s="8" t="n">
@@ -1384,7 +1384,7 @@
       </c>
       <c r="I38" s="10" t="inlineStr">
         <is>
-          <t>Фe3+</t>
+          <t>Qe3+</t>
         </is>
       </c>
     </row>
@@ -1394,12 +1394,12 @@
       </c>
       <c r="B39" s="10" t="inlineStr">
         <is>
-          <t>Ce5+</t>
+          <t>Be5+</t>
         </is>
       </c>
       <c r="C39" s="10" t="inlineStr">
         <is>
-          <t>Крb6</t>
+          <t>Kb6</t>
         </is>
       </c>
       <c r="G39" s="8" t="n">
@@ -1407,12 +1407,12 @@
       </c>
       <c r="H39" s="10" t="inlineStr">
         <is>
-          <t>Крh4</t>
+          <t>Kh4</t>
         </is>
       </c>
       <c r="I39" s="10" t="inlineStr">
         <is>
-          <t>Фxf4</t>
+          <t>Qxf4</t>
         </is>
       </c>
     </row>
@@ -1422,12 +1422,12 @@
       </c>
       <c r="B40" s="10" t="inlineStr">
         <is>
-          <t>Cd4+</t>
+          <t>Bd4+</t>
         </is>
       </c>
       <c r="C40" s="10" t="inlineStr">
         <is>
-          <t>Крc7</t>
+          <t>Kc7</t>
         </is>
       </c>
       <c r="G40" s="8" t="n">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="H40" s="10" t="inlineStr">
         <is>
-          <t>Крh5</t>
+          <t>Kh5</t>
         </is>
       </c>
       <c r="I40" s="10" t="inlineStr">
@@ -1450,12 +1450,12 @@
       </c>
       <c r="B41" s="10" t="inlineStr">
         <is>
-          <t>Cg7</t>
+          <t>Bg7</t>
         </is>
       </c>
       <c r="C41" s="10" t="inlineStr">
         <is>
-          <t>Лf7</t>
+          <t>Rf7</t>
         </is>
       </c>
       <c r="G41" s="8" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="H41" s="10" t="inlineStr">
         <is>
-          <t>Крh4</t>
+          <t>Kh4</t>
         </is>
       </c>
       <c r="I41" s="10" t="inlineStr">
@@ -1483,7 +1483,7 @@
       </c>
       <c r="C42" s="10" t="inlineStr">
         <is>
-          <t>Крd6</t>
+          <t>Kd6</t>
         </is>
       </c>
       <c r="G42" s="8" t="n">
@@ -1491,12 +1491,12 @@
       </c>
       <c r="H42" s="10" t="inlineStr">
         <is>
-          <t>Крh5</t>
+          <t>Kh5</t>
         </is>
       </c>
       <c r="I42" s="10" t="inlineStr">
         <is>
-          <t>Фg3</t>
+          <t>Qg3</t>
         </is>
       </c>
     </row>
@@ -1506,12 +1506,12 @@
       </c>
       <c r="B43" s="10" t="inlineStr">
         <is>
-          <t>Ca1</t>
+          <t>Ba1</t>
         </is>
       </c>
       <c r="C43" s="10" t="inlineStr">
         <is>
-          <t>Крxd5</t>
+          <t>Kxd5</t>
         </is>
       </c>
       <c r="G43" s="8" t="n">
@@ -1519,12 +1519,12 @@
       </c>
       <c r="H43" s="10" t="inlineStr">
         <is>
-          <t>Лd1</t>
+          <t>Rd1</t>
         </is>
       </c>
       <c r="I43" s="10" t="inlineStr">
         <is>
-          <t>Фxh3#</t>
+          <t>Qxh3#</t>
         </is>
       </c>
     </row>
@@ -1534,12 +1534,12 @@
       </c>
       <c r="B44" s="10" t="inlineStr">
         <is>
-          <t>Лh5</t>
+          <t>Rh5</t>
         </is>
       </c>
       <c r="C44" s="10" t="inlineStr">
         <is>
-          <t>Лe7</t>
+          <t>Re7</t>
         </is>
       </c>
       <c r="G44" s="8" t="n">
@@ -1550,16 +1550,6 @@
       <c r="A45" s="8" t="n">
         <v>34</v>
       </c>
-      <c r="B45" s="10" t="inlineStr">
-        <is>
-          <t>Лxh4</t>
-        </is>
-      </c>
-      <c r="C45" s="10" t="inlineStr">
-        <is>
-          <t>Лe2</t>
-        </is>
-      </c>
       <c r="G45" s="8" t="n">
         <v>34</v>
       </c>
@@ -1568,16 +1558,6 @@
       <c r="A46" s="8" t="n">
         <v>35</v>
       </c>
-      <c r="B46" s="10" t="inlineStr">
-        <is>
-          <t>Крg3</t>
-        </is>
-      </c>
-      <c r="C46" s="10" t="inlineStr">
-        <is>
-          <t>Лxa2</t>
-        </is>
-      </c>
       <c r="G46" s="8" t="n">
         <v>35</v>
       </c>
@@ -1585,16 +1565,6 @@
     <row r="47">
       <c r="A47" s="8" t="n">
         <v>36</v>
-      </c>
-      <c r="B47" s="10" t="inlineStr">
-        <is>
-          <t>Ch8</t>
-        </is>
-      </c>
-      <c r="C47" s="10" t="inlineStr">
-        <is>
-          <t>Лa3</t>
-        </is>
       </c>
       <c r="G47" s="8" t="n">
         <v>36</v>

</xml_diff>